<commit_message>
save notes to Lochlen's data cleaning file
</commit_message>
<xml_diff>
--- a/data/interim/cleaning_notes/Data cleaning  FNA and FoC SOLVED.xlsx
+++ b/data/interim/cleaning_notes/Data cleaning  FNA and FoC SOLVED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/carex-climate-morpho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/carex-climate-morpho/data/interim/cleaning_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3235C87D-376E-CF47-A67C-521F09F8F887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA71196-A5AB-854C-A366-36F73E518132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="1920" windowWidth="39440" windowHeight="23980" xr2:uid="{A30FD24B-2F2E-4070-9956-16D3C733C7AF}"/>
+    <workbookView xWindow="5120" yWindow="1320" windowWidth="35400" windowHeight="23480" xr2:uid="{A30FD24B-2F2E-4070-9956-16D3C733C7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t xml:space="preserve">FNA issues found in data collection </t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>Added achene_thickness as property to be included in dataset</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>You'll have to search for the multiplication symbol in the data and deal with it accordingly</t>
+  </si>
+  <si>
+    <t>atypical</t>
+  </si>
+  <si>
+    <t>inflorescence blade bract and leaf blade confusion</t>
+  </si>
+  <si>
+    <t>figure out how many times the inflorescence blade situation occurs and in which files</t>
+  </si>
+  <si>
+    <t>added subspecies and variety names to foc files</t>
   </si>
 </sst>
 </file>
@@ -1650,13 +1671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C231EB-5EFC-4E8A-A0AE-E9B55381CA5A}">
   <dimension ref="A2:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="J41" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1722,6 +1743,14 @@
       <c r="M8" t="s">
         <v>40</v>
       </c>
+      <c r="N8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I14">
@@ -1884,9 +1913,6 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="I53">
         <v>1</v>
       </c>
@@ -1909,11 +1935,22 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="M56" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="B59" t="s">
         <v>43</v>
       </c>
@@ -1924,14 +1961,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="B67" s="1" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +2008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>13</v>
       </c>
@@ -1975,20 +2025,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M70" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M71" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I73">
         <v>2</v>
       </c>

</xml_diff>